<commit_message>
Initial start to presentation
</commit_message>
<xml_diff>
--- a/shakespeare-stats.xlsx
+++ b/shakespeare-stats.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4712" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4714" uniqueCount="1144">
   <si>
     <t>Macbeth</t>
   </si>
@@ -3455,14 +3455,25 @@
   </si>
   <si>
     <t>Characters</t>
+  </si>
+  <si>
+    <t>Genre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3542,43 +3553,44 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3860,10 +3872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,18 +3884,52 @@
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>1141</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>1142</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="12" t="str">
+        <f>"&lt;tr class='headers'&gt;"</f>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H1" s="12" t="str">
+        <f>"&lt;th class='" &amp; LOWER(A$1) &amp; "'&gt;" &amp; A1 &amp; "&lt;/th&gt;"</f>
+        <v>&lt;th class='play'&gt;Play&lt;/th&gt;</v>
+      </c>
+      <c r="I1" s="12" t="str">
+        <f t="shared" ref="I1:L1" si="0">"&lt;th class='" &amp; LOWER(B$1) &amp; "'&gt;" &amp; B1 &amp; "&lt;/th&gt;"</f>
+        <v>&lt;th class='genre'&gt;Genre&lt;/th&gt;</v>
+      </c>
+      <c r="J1" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;th class='searches'&gt;Searches&lt;/th&gt;</v>
+      </c>
+      <c r="K1" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;th class='characters'&gt;Characters&lt;/th&gt;</v>
+      </c>
+      <c r="L1" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;th class='lines'&gt;Lines&lt;/th&gt;</v>
+      </c>
+      <c r="M1" s="12" t="str">
+        <f>"&lt;/tr&gt;"</f>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3901,8 +3947,36 @@
         <f>SUMIF(Characters!B:B,Table!A2,Characters!D:D)</f>
         <v>2361</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="12" t="str">
+        <f>"&lt;tr class='headers'&gt;"</f>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H2" s="12" t="str">
+        <f>"&lt;td class='" &amp; LOWER(A$1) &amp; "'&gt;&lt;a href='http://www.shakespeareswords.com/" &amp; SUBSTITUTE(SUBSTITUTE(A2,"'", "")," ","-") &amp; "'&gt;" &amp; A2 &amp; "&lt;/a&gt;&lt;/td&gt;"</f>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/Macbeth'&gt;Macbeth&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I2" s="12" t="str">
+        <f t="shared" ref="I2:I11" si="1">"&lt;td class='" &amp; LOWER(B$1) &amp; "'&gt;" &amp; B2 &amp; "&lt;/td&gt;"</f>
+        <v>&lt;td class='genre'&gt;Tragedy&lt;/td&gt;</v>
+      </c>
+      <c r="J2" s="12" t="str">
+        <f t="shared" ref="J2:J11" si="2">"&lt;td class='" &amp; LOWER(C$1) &amp; "'&gt;" &amp; C2 &amp; "&lt;/td&gt;"</f>
+        <v>&lt;td class='searches'&gt;245837&lt;/td&gt;</v>
+      </c>
+      <c r="K2" s="12" t="str">
+        <f t="shared" ref="K2:K11" si="3">"&lt;td class='" &amp; LOWER(D$1) &amp; "'&gt;" &amp; D2 &amp; "&lt;/td&gt;"</f>
+        <v>&lt;td class='characters'&gt;45&lt;/td&gt;</v>
+      </c>
+      <c r="L2" s="12" t="str">
+        <f t="shared" ref="L2:L11" si="4">"&lt;td class='" &amp; LOWER(E$1) &amp; "'&gt;" &amp; E2 &amp; "&lt;/td&gt;"</f>
+        <v>&lt;td class='lines'&gt;2361&lt;/td&gt;</v>
+      </c>
+      <c r="M2" s="12" t="str">
+        <f>"&lt;/tr&gt;"</f>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3920,8 +3994,36 @@
         <f>SUMIF(Characters!B:B,Table!A3,Characters!D:D)</f>
         <v>4051</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="12" t="str">
+        <f t="shared" ref="G3:G11" si="5">"&lt;tr class='headers'&gt;"</f>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H3" s="12" t="str">
+        <f t="shared" ref="H3:H11" si="6">"&lt;td class='" &amp; LOWER(A$1) &amp; "'&gt;&lt;a href='http://www.shakespeareswords.com/" &amp; SUBSTITUTE(SUBSTITUTE(A3,"'", "")," ","-") &amp; "'&gt;" &amp; A3 &amp; "&lt;/a&gt;&lt;/td&gt;"</f>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/Hamlet'&gt;Hamlet&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I3" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Tragedy&lt;/td&gt;</v>
+      </c>
+      <c r="J3" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;216964&lt;/td&gt;</v>
+      </c>
+      <c r="K3" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;39&lt;/td&gt;</v>
+      </c>
+      <c r="L3" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;4051&lt;/td&gt;</v>
+      </c>
+      <c r="M3" s="12" t="str">
+        <f t="shared" ref="M3:M11" si="7">"&lt;/tr&gt;"</f>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3939,8 +4041,36 @@
         <f>SUMIF(Characters!B:B,Table!A4,Characters!D:D)</f>
         <v>3098</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H4" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/Romeo-and-Juliet'&gt;Romeo and Juliet&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I4" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Tragedy&lt;/td&gt;</v>
+      </c>
+      <c r="J4" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;180041&lt;/td&gt;</v>
+      </c>
+      <c r="K4" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;42&lt;/td&gt;</v>
+      </c>
+      <c r="L4" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;3098&lt;/td&gt;</v>
+      </c>
+      <c r="M4" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3958,8 +4088,36 @@
         <f>SUMIF(Characters!B:B,Table!A5,Characters!D:D)</f>
         <v>3542</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H5" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/Othello'&gt;Othello&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I5" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Tragedy&lt;/td&gt;</v>
+      </c>
+      <c r="J5" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;128244&lt;/td&gt;</v>
+      </c>
+      <c r="K5" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;29&lt;/td&gt;</v>
+      </c>
+      <c r="L5" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;3542&lt;/td&gt;</v>
+      </c>
+      <c r="M5" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3977,8 +4135,36 @@
         <f>SUMIF(Characters!B:B,Table!A6,Characters!D:D)</f>
         <v>3469</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H6" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/King-Lear'&gt;King Lear&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I6" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Tragedy&lt;/td&gt;</v>
+      </c>
+      <c r="J6" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;106605&lt;/td&gt;</v>
+      </c>
+      <c r="K6" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;27&lt;/td&gt;</v>
+      </c>
+      <c r="L6" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;3469&lt;/td&gt;</v>
+      </c>
+      <c r="M6" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>194</v>
       </c>
@@ -3996,8 +4182,36 @@
         <f>SUMIF(Characters!B:B,Table!A7,Characters!D:D)</f>
         <v>2165</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H7" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/A-Midsummer-Nights-Dream'&gt;A Midsummer Night's Dream&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I7" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Comedy&lt;/td&gt;</v>
+      </c>
+      <c r="J7" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;82476&lt;/td&gt;</v>
+      </c>
+      <c r="K7" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;27&lt;/td&gt;</v>
+      </c>
+      <c r="L7" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;2165&lt;/td&gt;</v>
+      </c>
+      <c r="M7" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -4015,8 +4229,36 @@
         <f>SUMIF(Characters!B:B,Table!A8,Characters!D:D)</f>
         <v>2533</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H8" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/Twelfth-Night'&gt;Twelfth Night&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I8" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Comedy&lt;/td&gt;</v>
+      </c>
+      <c r="J8" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;61552&lt;/td&gt;</v>
+      </c>
+      <c r="K8" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;18&lt;/td&gt;</v>
+      </c>
+      <c r="L8" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;2533&lt;/td&gt;</v>
+      </c>
+      <c r="M8" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>88</v>
       </c>
@@ -4034,8 +4276,36 @@
         <f>SUMIF(Characters!B:B,Table!A9,Characters!D:D)</f>
         <v>2660</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H9" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/The-Merchant-of-Venice'&gt;The Merchant of Venice&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I9" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Comedy&lt;/td&gt;</v>
+      </c>
+      <c r="J9" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;58923&lt;/td&gt;</v>
+      </c>
+      <c r="K9" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;25&lt;/td&gt;</v>
+      </c>
+      <c r="L9" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;2660&lt;/td&gt;</v>
+      </c>
+      <c r="M9" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>74</v>
       </c>
@@ -4053,8 +4323,36 @@
         <f>SUMIF(Characters!B:B,Table!A10,Characters!D:D)</f>
         <v>2284</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H10" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/The-Tempest'&gt;The Tempest&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I10" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Comedy&lt;/td&gt;</v>
+      </c>
+      <c r="J10" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;57533&lt;/td&gt;</v>
+      </c>
+      <c r="K10" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;20&lt;/td&gt;</v>
+      </c>
+      <c r="L10" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;2284&lt;/td&gt;</v>
+      </c>
+      <c r="M10" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -4072,9 +4370,38 @@
         <f>SUMIF(Characters!B:B,Table!A11,Characters!D:D)</f>
         <v>2648</v>
       </c>
+      <c r="G11" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='headers'&gt;</v>
+      </c>
+      <c r="H11" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td class='play'&gt;&lt;a href='http://www.shakespeareswords.com/Much-Ado-about-Nothing'&gt;Much Ado about Nothing&lt;/a&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="I11" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;td class='genre'&gt;Comedy&lt;/td&gt;</v>
+      </c>
+      <c r="J11" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td class='searches'&gt;56800&lt;/td&gt;</v>
+      </c>
+      <c r="K11" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='characters'&gt;23&lt;/td&gt;</v>
+      </c>
+      <c r="L11" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='lines'&gt;2648&lt;/td&gt;</v>
+      </c>
+      <c r="M11" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/tr&gt;</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>